<commit_message>
update code and docs
</commit_message>
<xml_diff>
--- a/zone/notebook/Tests/lift test 1.xlsx
+++ b/zone/notebook/Tests/lift test 1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robbie Buxton\Documents\GitHub\Fortismere-Vex-EDR-2017-2017\zone\notebook\Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\Fortismere-Vex-EDR\zone\notebook\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,21 +24,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Number of cones</t>
+    <t xml:space="preserve">Number of Cones </t>
   </si>
   <si>
-    <t>N/A</t>
+    <t>No bands</t>
   </si>
   <si>
-    <t>Success/Failure</t>
+    <t>Two bands</t>
   </si>
   <si>
-    <t>Weight (Kg)</t>
+    <t>Four Bands</t>
   </si>
   <si>
-    <t>Success</t>
+    <t>Six bands</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -62,18 +65,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -88,9 +85,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -406,168 +402,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1.4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1.5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1.6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1.7</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1.8</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1.9</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2.1</v>
-      </c>
-      <c r="B9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="B11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2.4</v>
-      </c>
-      <c r="B12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2.5</v>
-      </c>
-      <c r="B13">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2.6</v>
-      </c>
-      <c r="B14" s="1">
-        <v>8</v>
-      </c>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2.7</v>
-      </c>
-      <c r="B15">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2.8</v>
-      </c>
-      <c r="B16">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2.9</v>
-      </c>
-      <c r="B17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>3</v>
-      </c>
-      <c r="B18">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>